<commit_message>
Add UtilityLink currentStatus in Codelist Usage
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_Codelists.xlsx
+++ b/implementation/Documentation/IMKL3_Codelists.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\IMKL 3\Implementatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\Belgif\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA04D52-903B-42FF-BF46-D294E7FA98CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52998FE-8173-40AA-8DEC-66C7FDA61F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" activeTab="1" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="860">
   <si>
     <t>nilReason</t>
   </si>
@@ -2632,6 +2632,9 @@
   </si>
   <si>
     <t>E.g. cables used to convey data.</t>
+  </si>
+  <si>
+    <t>UtilityLink</t>
   </si>
 </sst>
 </file>
@@ -3094,7 +3097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12F05A2-F84B-4BFA-ADF4-7302F1870D77}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -3976,10 +3979,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64294C56-C363-4325-A21C-BEAD7C56353B}">
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6312,6 +6315,21 @@
       <c r="D155" t="str">
         <f>VLOOKUP(C155,Overview!B:B,1,0)</f>
         <v>WaterTypeValue</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>859</v>
+      </c>
+      <c r="B156" t="s">
+        <v>593</v>
+      </c>
+      <c r="C156" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" t="str">
+        <f>VLOOKUP(C156,Overview!B:B,1,0)</f>
+        <v>ConditionOfFacilityValue</v>
       </c>
     </row>
   </sheetData>
@@ -6335,7 +6353,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13809,6 +13827,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -14068,16 +14095,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791B434E-C5B6-43DF-B218-859297235BBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14095,12 +14121,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix typo with ElectricityCable
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_Codelists.xlsx
+++ b/implementation/Documentation/IMKL3_Codelists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\Belgif\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFA2361-FA15-403A-A1BD-FA99126767B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38EFE85-2487-46B2-AC94-499FC00615DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16332" yWindow="5688" windowWidth="34560" windowHeight="22452" activeTab="1" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
@@ -3982,7 +3982,7 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Added inSharedContainer property and updated documentation
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_Codelists.xlsx
+++ b/implementation/Documentation/IMKL3_Codelists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E46885-E336-4888-B931-B1B61364A650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA09841-84DA-42F7-BF42-CD23ED9BC078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="30480" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="17268" yWindow="3096" windowWidth="26196" windowHeight="25128" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -4019,7 +4019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12F05A2-F84B-4BFA-ADF4-7302F1870D77}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
@@ -7364,11 +7364,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H258" sqref="H258"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C263" sqref="C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8222,7 +8223,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" hidden="1">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" hidden="1">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -8282,7 +8283,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" hidden="1">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" hidden="1">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -8342,7 +8343,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" hidden="1">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -8372,7 +8373,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" hidden="1">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -8402,7 +8403,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" hidden="1">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -8432,7 +8433,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" hidden="1">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -8462,7 +8463,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" hidden="1">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -8492,7 +8493,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" hidden="1">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" hidden="1">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -8552,7 +8553,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" hidden="1">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -8582,7 +8583,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" hidden="1">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -8612,7 +8613,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" hidden="1">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -8642,7 +8643,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" hidden="1">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -8672,7 +8673,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" hidden="1">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -8702,7 +8703,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" hidden="1">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -8729,7 +8730,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" hidden="1">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -8759,7 +8760,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" hidden="1">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -8789,7 +8790,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" hidden="1">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -8819,7 +8820,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -8849,7 +8850,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -8879,7 +8880,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -8909,7 +8910,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" hidden="1">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -8939,7 +8940,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -8969,7 +8970,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -8999,7 +9000,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" hidden="1">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -9029,7 +9030,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" hidden="1">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -9059,7 +9060,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" hidden="1">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -9089,7 +9090,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -9119,7 +9120,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" hidden="1">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -9149,7 +9150,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" hidden="1">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -9179,7 +9180,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" hidden="1">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -9209,7 +9210,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" hidden="1">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -9239,7 +9240,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -9269,7 +9270,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" hidden="1">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -9299,7 +9300,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" hidden="1">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -9329,7 +9330,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" hidden="1">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -9359,7 +9360,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" hidden="1">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -9389,7 +9390,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" hidden="1">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -9419,7 +9420,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" hidden="1">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -9449,7 +9450,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" hidden="1">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -9479,7 +9480,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" hidden="1">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -9509,7 +9510,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" hidden="1">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" hidden="1">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -9569,7 +9570,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" hidden="1">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -9599,7 +9600,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" hidden="1">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -9629,7 +9630,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" hidden="1">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -9659,7 +9660,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" hidden="1">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -9689,7 +9690,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" hidden="1">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -9719,7 +9720,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" hidden="1">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" hidden="1">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -9779,7 +9780,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" hidden="1">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -9809,7 +9810,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" hidden="1">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" hidden="1">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -9869,7 +9870,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" hidden="1">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -9899,7 +9900,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" hidden="1">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -9929,7 +9930,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" hidden="1">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -9959,7 +9960,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" hidden="1">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -9989,7 +9990,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" hidden="1">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -10019,7 +10020,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" hidden="1">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -10049,7 +10050,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" hidden="1">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -10079,7 +10080,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" hidden="1">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -10109,7 +10110,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" hidden="1">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" hidden="1">
       <c r="A93" t="s">
         <v>135</v>
       </c>
@@ -10169,7 +10170,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" hidden="1">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -10199,7 +10200,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" hidden="1">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -10229,7 +10230,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" hidden="1">
       <c r="A96" t="s">
         <v>139</v>
       </c>
@@ -10259,7 +10260,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" hidden="1">
       <c r="A97" t="s">
         <v>139</v>
       </c>
@@ -10289,7 +10290,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" hidden="1">
       <c r="A98" t="s">
         <v>139</v>
       </c>
@@ -10319,7 +10320,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" hidden="1">
       <c r="A99" t="s">
         <v>139</v>
       </c>
@@ -10349,7 +10350,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" hidden="1">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -10379,7 +10380,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" hidden="1">
       <c r="A101" t="s">
         <v>139</v>
       </c>
@@ -10409,7 +10410,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" hidden="1">
       <c r="A102" t="s">
         <v>139</v>
       </c>
@@ -10439,7 +10440,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" hidden="1">
       <c r="A103" t="s">
         <v>139</v>
       </c>
@@ -10469,7 +10470,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" hidden="1">
       <c r="A104" t="s">
         <v>139</v>
       </c>
@@ -10499,7 +10500,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" hidden="1">
       <c r="A105" t="s">
         <v>139</v>
       </c>
@@ -10529,7 +10530,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" hidden="1">
       <c r="A106" t="s">
         <v>139</v>
       </c>
@@ -10559,7 +10560,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" hidden="1">
       <c r="A107" t="s">
         <v>152</v>
       </c>
@@ -10589,7 +10590,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" hidden="1">
       <c r="A108" t="s">
         <v>152</v>
       </c>
@@ -10619,7 +10620,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" hidden="1">
       <c r="A109" t="s">
         <v>152</v>
       </c>
@@ -10649,7 +10650,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" hidden="1">
       <c r="A110" t="s">
         <v>152</v>
       </c>
@@ -10679,7 +10680,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" hidden="1">
       <c r="A111" t="s">
         <v>152</v>
       </c>
@@ -10709,7 +10710,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" hidden="1">
       <c r="A112" t="s">
         <v>152</v>
       </c>
@@ -10739,7 +10740,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" hidden="1">
       <c r="A113" t="s">
         <v>152</v>
       </c>
@@ -10769,7 +10770,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" hidden="1">
       <c r="A114" t="s">
         <v>152</v>
       </c>
@@ -10799,7 +10800,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" hidden="1">
       <c r="A115" t="s">
         <v>152</v>
       </c>
@@ -10829,7 +10830,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" hidden="1">
       <c r="A116" t="s">
         <v>155</v>
       </c>
@@ -10859,7 +10860,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" hidden="1">
       <c r="A117" t="s">
         <v>155</v>
       </c>
@@ -10889,7 +10890,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" hidden="1">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -10919,7 +10920,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" hidden="1">
       <c r="A119" t="s">
         <v>155</v>
       </c>
@@ -10949,7 +10950,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" hidden="1">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -10979,7 +10980,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" hidden="1">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -11009,7 +11010,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" hidden="1">
       <c r="A122" t="s">
         <v>323</v>
       </c>
@@ -11039,7 +11040,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" hidden="1">
       <c r="A123" t="s">
         <v>158</v>
       </c>
@@ -11069,7 +11070,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" hidden="1">
       <c r="A124" t="s">
         <v>160</v>
       </c>
@@ -11099,7 +11100,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" hidden="1">
       <c r="A125" t="s">
         <v>160</v>
       </c>
@@ -11129,7 +11130,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" hidden="1">
       <c r="A126" t="s">
         <v>160</v>
       </c>
@@ -11159,7 +11160,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" hidden="1">
       <c r="A127" t="s">
         <v>160</v>
       </c>
@@ -11189,7 +11190,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" hidden="1">
       <c r="A128" t="s">
         <v>160</v>
       </c>
@@ -11219,7 +11220,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" hidden="1">
       <c r="A129" t="s">
         <v>160</v>
       </c>
@@ -11249,7 +11250,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" hidden="1">
       <c r="A130" t="s">
         <v>160</v>
       </c>
@@ -11279,7 +11280,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" hidden="1">
       <c r="A131" t="s">
         <v>160</v>
       </c>
@@ -11309,7 +11310,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" hidden="1">
       <c r="A132" t="s">
         <v>160</v>
       </c>
@@ -11339,7 +11340,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" hidden="1">
       <c r="A133" t="s">
         <v>160</v>
       </c>
@@ -11369,7 +11370,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" hidden="1">
       <c r="A134" t="s">
         <v>160</v>
       </c>
@@ -11399,7 +11400,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" hidden="1">
       <c r="A135" t="s">
         <v>160</v>
       </c>
@@ -11429,7 +11430,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" hidden="1">
       <c r="A136" t="s">
         <v>160</v>
       </c>
@@ -11459,7 +11460,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" hidden="1">
       <c r="A137" t="s">
         <v>160</v>
       </c>
@@ -11489,7 +11490,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" hidden="1">
       <c r="A138" t="s">
         <v>160</v>
       </c>
@@ -11519,7 +11520,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" hidden="1">
       <c r="A139" t="s">
         <v>160</v>
       </c>
@@ -11549,7 +11550,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" hidden="1">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -11579,7 +11580,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" hidden="1">
       <c r="A141" t="s">
         <v>161</v>
       </c>
@@ -11609,7 +11610,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" hidden="1">
       <c r="A142" t="s">
         <v>161</v>
       </c>
@@ -11639,7 +11640,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" hidden="1">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -11669,7 +11670,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" hidden="1">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -11699,7 +11700,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" hidden="1">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -11729,7 +11730,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" hidden="1">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -11759,7 +11760,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" hidden="1">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -11789,7 +11790,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" hidden="1">
       <c r="A148" t="s">
         <v>161</v>
       </c>
@@ -11819,7 +11820,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" hidden="1">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -11849,7 +11850,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" hidden="1">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -11879,7 +11880,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" hidden="1">
       <c r="A151" t="s">
         <v>161</v>
       </c>
@@ -11909,7 +11910,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" hidden="1">
       <c r="A152" t="s">
         <v>161</v>
       </c>
@@ -11939,7 +11940,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" hidden="1">
       <c r="A153" t="s">
         <v>161</v>
       </c>
@@ -11969,7 +11970,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" hidden="1">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -11999,7 +12000,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" hidden="1">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -12029,7 +12030,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" hidden="1">
       <c r="A156" t="s">
         <v>161</v>
       </c>
@@ -12059,7 +12060,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" hidden="1">
       <c r="A157" t="s">
         <v>161</v>
       </c>
@@ -12089,7 +12090,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" hidden="1">
       <c r="A158" t="s">
         <v>161</v>
       </c>
@@ -12119,7 +12120,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" hidden="1">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -12149,7 +12150,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" hidden="1">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -12179,7 +12180,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" hidden="1">
       <c r="A161" t="s">
         <v>161</v>
       </c>
@@ -12209,7 +12210,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" hidden="1">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -12239,7 +12240,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" hidden="1">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -12269,7 +12270,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" hidden="1">
       <c r="A164" t="s">
         <v>161</v>
       </c>
@@ -12299,7 +12300,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" hidden="1">
       <c r="A165" t="s">
         <v>170</v>
       </c>
@@ -12329,7 +12330,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" hidden="1">
       <c r="A166" t="s">
         <v>170</v>
       </c>
@@ -12359,7 +12360,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" hidden="1">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -12389,7 +12390,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" hidden="1">
       <c r="A168" t="s">
         <v>338</v>
       </c>
@@ -12419,7 +12420,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" hidden="1">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -12449,7 +12450,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" hidden="1">
       <c r="A170" t="s">
         <v>338</v>
       </c>
@@ -12479,7 +12480,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" hidden="1">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -12509,7 +12510,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" hidden="1">
       <c r="A172" t="s">
         <v>327</v>
       </c>
@@ -12539,7 +12540,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" hidden="1">
       <c r="A173" t="s">
         <v>327</v>
       </c>
@@ -12569,7 +12570,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" hidden="1">
       <c r="A174" t="s">
         <v>327</v>
       </c>
@@ -12599,7 +12600,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" hidden="1">
       <c r="A175" t="s">
         <v>327</v>
       </c>
@@ -12629,7 +12630,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" hidden="1">
       <c r="A176" t="s">
         <v>325</v>
       </c>
@@ -12659,7 +12660,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" hidden="1">
       <c r="A177" t="s">
         <v>325</v>
       </c>
@@ -12689,7 +12690,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" hidden="1">
       <c r="A178" t="s">
         <v>325</v>
       </c>
@@ -12719,7 +12720,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" hidden="1">
       <c r="A179" t="s">
         <v>325</v>
       </c>
@@ -12749,7 +12750,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" hidden="1">
       <c r="A180" t="s">
         <v>320</v>
       </c>
@@ -12779,7 +12780,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" hidden="1">
       <c r="A181" t="s">
         <v>320</v>
       </c>
@@ -12809,7 +12810,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" hidden="1">
       <c r="A182" t="s">
         <v>320</v>
       </c>
@@ -12839,7 +12840,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" hidden="1">
       <c r="A183" t="s">
         <v>320</v>
       </c>
@@ -12869,7 +12870,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" hidden="1">
       <c r="A184" t="s">
         <v>341</v>
       </c>
@@ -12899,7 +12900,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="28.8">
+    <row r="185" spans="1:9" ht="28.8" hidden="1">
       <c r="A185" t="s">
         <v>323</v>
       </c>
@@ -12929,7 +12930,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" hidden="1">
       <c r="A186" t="s">
         <v>158</v>
       </c>
@@ -12959,7 +12960,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="57.6">
+    <row r="187" spans="1:9" ht="57.6" hidden="1">
       <c r="A187" t="s">
         <v>323</v>
       </c>
@@ -12989,7 +12990,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" hidden="1">
       <c r="A188" t="s">
         <v>315</v>
       </c>
@@ -13019,7 +13020,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" hidden="1">
       <c r="A189" t="s">
         <v>315</v>
       </c>
@@ -13049,7 +13050,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" hidden="1">
       <c r="A190" t="s">
         <v>316</v>
       </c>
@@ -13079,7 +13080,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" hidden="1">
       <c r="A191" t="s">
         <v>316</v>
       </c>
@@ -13109,7 +13110,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" hidden="1">
       <c r="A192" t="s">
         <v>316</v>
       </c>
@@ -13139,7 +13140,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" hidden="1">
       <c r="A193" t="s">
         <v>317</v>
       </c>
@@ -13169,7 +13170,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" hidden="1">
       <c r="A194" t="s">
         <v>317</v>
       </c>
@@ -13199,7 +13200,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" hidden="1">
       <c r="A195" t="s">
         <v>152</v>
       </c>
@@ -13229,7 +13230,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" hidden="1">
       <c r="A196" t="s">
         <v>317</v>
       </c>
@@ -13259,7 +13260,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" hidden="1">
       <c r="A197" t="s">
         <v>317</v>
       </c>
@@ -13289,7 +13290,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" hidden="1">
       <c r="A198" t="s">
         <v>317</v>
       </c>
@@ -13319,7 +13320,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" hidden="1">
       <c r="A199" t="s">
         <v>318</v>
       </c>
@@ -13349,7 +13350,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" hidden="1">
       <c r="A200" t="s">
         <v>318</v>
       </c>
@@ -13379,7 +13380,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" hidden="1">
       <c r="A201" t="s">
         <v>318</v>
       </c>
@@ -13409,7 +13410,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" hidden="1">
       <c r="A202" t="s">
         <v>318</v>
       </c>
@@ -13439,7 +13440,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" hidden="1">
       <c r="A203" t="s">
         <v>318</v>
       </c>
@@ -13469,7 +13470,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" hidden="1">
       <c r="A204" t="s">
         <v>318</v>
       </c>
@@ -13499,7 +13500,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" hidden="1">
       <c r="A205" t="s">
         <v>318</v>
       </c>
@@ -13529,7 +13530,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" hidden="1">
       <c r="A206" t="s">
         <v>318</v>
       </c>
@@ -13559,7 +13560,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" hidden="1">
       <c r="A207" t="s">
         <v>318</v>
       </c>
@@ -13589,7 +13590,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" hidden="1">
       <c r="A208" t="s">
         <v>318</v>
       </c>
@@ -13619,7 +13620,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" hidden="1">
       <c r="A209" t="s">
         <v>318</v>
       </c>
@@ -13649,7 +13650,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" hidden="1">
       <c r="A210" t="s">
         <v>170</v>
       </c>
@@ -13679,7 +13680,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" hidden="1">
       <c r="A211" t="s">
         <v>170</v>
       </c>
@@ -13709,7 +13710,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" hidden="1">
       <c r="A212" t="s">
         <v>322</v>
       </c>
@@ -13739,7 +13740,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" hidden="1">
       <c r="A213" t="s">
         <v>322</v>
       </c>
@@ -13769,7 +13770,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" hidden="1">
       <c r="A214" t="s">
         <v>322</v>
       </c>
@@ -13799,7 +13800,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" hidden="1">
       <c r="A215" t="s">
         <v>322</v>
       </c>
@@ -13829,7 +13830,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" hidden="1">
       <c r="A216" t="s">
         <v>322</v>
       </c>
@@ -13859,7 +13860,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" hidden="1">
       <c r="A217" t="s">
         <v>322</v>
       </c>
@@ -13889,7 +13890,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" hidden="1">
       <c r="A218" t="s">
         <v>340</v>
       </c>
@@ -13919,7 +13920,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" hidden="1">
       <c r="A219" t="s">
         <v>173</v>
       </c>
@@ -13949,7 +13950,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" hidden="1">
       <c r="A220" t="s">
         <v>173</v>
       </c>
@@ -13979,7 +13980,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" hidden="1">
       <c r="A221" t="s">
         <v>173</v>
       </c>
@@ -14009,7 +14010,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" hidden="1">
       <c r="A222" t="s">
         <v>6</v>
       </c>
@@ -14039,7 +14040,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" hidden="1">
       <c r="A223" t="s">
         <v>6</v>
       </c>
@@ -14069,7 +14070,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" hidden="1">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -14099,7 +14100,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" hidden="1">
       <c r="A225" t="s">
         <v>6</v>
       </c>
@@ -14129,7 +14130,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" hidden="1">
       <c r="A226" t="s">
         <v>241</v>
       </c>
@@ -14159,7 +14160,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" hidden="1">
       <c r="A227" t="s">
         <v>241</v>
       </c>
@@ -14189,7 +14190,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" hidden="1">
       <c r="A228" t="s">
         <v>241</v>
       </c>
@@ -14219,7 +14220,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" hidden="1">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -14240,7 +14241,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" hidden="1">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -14261,7 +14262,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" hidden="1">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -14282,7 +14283,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" hidden="1">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -14303,7 +14304,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" hidden="1">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -14324,7 +14325,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" hidden="1">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -14354,7 +14355,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" hidden="1">
       <c r="A235" t="s">
         <v>10</v>
       </c>
@@ -14384,7 +14385,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" hidden="1">
       <c r="A236" t="s">
         <v>10</v>
       </c>
@@ -14414,7 +14415,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" hidden="1">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -14444,7 +14445,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" hidden="1">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -14474,7 +14475,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" hidden="1">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -14504,7 +14505,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" hidden="1">
       <c r="A240" t="s">
         <v>10</v>
       </c>
@@ -14534,7 +14535,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" hidden="1">
       <c r="A241" t="s">
         <v>10</v>
       </c>
@@ -14564,7 +14565,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" hidden="1">
       <c r="A242" t="s">
         <v>10</v>
       </c>
@@ -14594,7 +14595,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" hidden="1">
       <c r="A243" t="s">
         <v>10</v>
       </c>
@@ -14624,7 +14625,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" hidden="1">
       <c r="A244" t="s">
         <v>8</v>
       </c>
@@ -14654,7 +14655,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" hidden="1">
       <c r="A245" t="s">
         <v>8</v>
       </c>
@@ -14684,7 +14685,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" hidden="1">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -14714,7 +14715,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" hidden="1">
       <c r="A247" t="s">
         <v>258</v>
       </c>
@@ -14744,7 +14745,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" hidden="1">
       <c r="A248" t="s">
         <v>258</v>
       </c>
@@ -14774,7 +14775,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" hidden="1">
       <c r="A249" t="s">
         <v>258</v>
       </c>
@@ -14804,7 +14805,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" hidden="1">
       <c r="A250" t="s">
         <v>258</v>
       </c>
@@ -14835,7 +14836,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}"/>
+  <autoFilter ref="A1:I250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ElectricitySubthemeValue"/>
+        <filter val="OilGasChemicalsSubthemeValue"/>
+        <filter val="SewerSubthemeValue"/>
+        <filter val="TelecommunicationsSubthemeValue"/>
+        <filter val="ThermalSubthemeValue"/>
+        <filter val="WaterSubthemeValue"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="H180" r:id="rId1" xr:uid="{937649D5-206B-4F0F-AC39-B248CB8B3379}"/>
     <hyperlink ref="H215" r:id="rId2" xr:uid="{58EA29A0-45FB-4990-9EF7-62E6622DF2D7}"/>
@@ -14895,15 +14907,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -15163,15 +15166,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791B434E-C5B6-43DF-B218-859297235BBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15189,4 +15193,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Dutch translation for codelist labels
</commit_message>
<xml_diff>
--- a/implementation/Documentation/IMKL3_Codelists.xlsx
+++ b/implementation/Documentation/IMKL3_Codelists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Athumi\ICEGthema-imkl\implementation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA09841-84DA-42F7-BF42-CD23ED9BC078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA144781-5675-49CA-8E45-7D224E651487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17268" yWindow="3096" windowWidth="26196" windowHeight="25128" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
+    <workbookView xWindow="23040" yWindow="0" windowWidth="23040" windowHeight="30264" activeTab="2" xr2:uid="{7D7764BC-E929-422B-98A1-10C145692BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="1167">
   <si>
     <t>nilReason</t>
   </si>
@@ -3550,6 +3550,12 @@
   </si>
   <si>
     <t>http://inspire.ec.europa.eu/codelist/VerticalPositionValue</t>
+  </si>
+  <si>
+    <t>Huisaansluiting</t>
+  </si>
+  <si>
+    <t>Coaxkabel</t>
   </si>
 </sst>
 </file>
@@ -7364,19 +7370,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C263" sqref="C263"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K176" sqref="K176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="45.109375" customWidth="1"/>
     <col min="2" max="2" width="21.109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" customWidth="1"/>
     <col min="6" max="6" width="56.5546875" customWidth="1"/>
@@ -8223,7 +8228,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -8253,7 +8258,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -8283,7 +8288,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -8313,7 +8318,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -8343,7 +8348,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -8373,7 +8378,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -8403,7 +8408,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -8433,7 +8438,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -8463,7 +8468,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -8493,7 +8498,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -8523,7 +8528,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -8553,7 +8558,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -8583,7 +8588,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -8613,7 +8618,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -8643,7 +8648,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -8673,7 +8678,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -8703,7 +8708,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -8730,7 +8735,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -8760,7 +8765,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -8790,7 +8795,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -8820,7 +8825,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -8850,7 +8855,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -8880,7 +8885,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -8910,7 +8915,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -8940,7 +8945,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -9000,7 +9005,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -9030,7 +9035,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -9060,7 +9065,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -9090,7 +9095,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -9120,7 +9125,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -9150,7 +9155,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -9180,7 +9185,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -9210,7 +9215,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -9240,7 +9245,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -9270,7 +9275,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -9300,7 +9305,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -9330,7 +9335,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -9360,7 +9365,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -9390,7 +9395,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -9420,7 +9425,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -9480,7 +9485,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -9510,7 +9515,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -9540,7 +9545,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -9570,7 +9575,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -9600,7 +9605,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -9630,7 +9635,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -9660,7 +9665,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -9690,7 +9695,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -9720,7 +9725,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -9750,7 +9755,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -9780,7 +9785,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -9810,7 +9815,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -9840,7 +9845,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -9870,7 +9875,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -9900,7 +9905,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -9930,7 +9935,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -9960,7 +9965,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -9990,7 +9995,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -10020,7 +10025,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -10050,7 +10055,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -10080,7 +10085,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -10110,7 +10115,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -10140,7 +10145,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>135</v>
       </c>
@@ -10170,7 +10175,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -10200,7 +10205,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -10230,7 +10235,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>139</v>
       </c>
@@ -10260,7 +10265,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>139</v>
       </c>
@@ -10290,7 +10295,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>139</v>
       </c>
@@ -10320,7 +10325,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>139</v>
       </c>
@@ -10350,7 +10355,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>139</v>
       </c>
@@ -10380,7 +10385,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>139</v>
       </c>
@@ -10410,7 +10415,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>139</v>
       </c>
@@ -10440,7 +10445,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>139</v>
       </c>
@@ -10470,7 +10475,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>139</v>
       </c>
@@ -10500,7 +10505,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>139</v>
       </c>
@@ -10530,7 +10535,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1">
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>139</v>
       </c>
@@ -10560,7 +10565,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1">
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>152</v>
       </c>
@@ -10590,7 +10595,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>152</v>
       </c>
@@ -10620,7 +10625,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1">
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>152</v>
       </c>
@@ -10650,7 +10655,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1">
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>152</v>
       </c>
@@ -10680,7 +10685,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1">
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>152</v>
       </c>
@@ -10710,7 +10715,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1">
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>152</v>
       </c>
@@ -10740,7 +10745,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1">
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>152</v>
       </c>
@@ -10770,7 +10775,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1">
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>152</v>
       </c>
@@ -10800,7 +10805,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1">
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>152</v>
       </c>
@@ -10830,7 +10835,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1">
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>155</v>
       </c>
@@ -10860,7 +10865,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1">
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>155</v>
       </c>
@@ -10890,7 +10895,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1">
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -10920,7 +10925,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1">
+    <row r="119" spans="1:9">
       <c r="A119" t="s">
         <v>155</v>
       </c>
@@ -10950,7 +10955,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1">
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -10980,7 +10985,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1">
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -11010,7 +11015,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1">
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>323</v>
       </c>
@@ -11040,7 +11045,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1">
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>158</v>
       </c>
@@ -11070,7 +11075,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1">
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>160</v>
       </c>
@@ -11100,7 +11105,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1">
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>160</v>
       </c>
@@ -11130,7 +11135,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1">
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>160</v>
       </c>
@@ -11160,7 +11165,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1">
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>160</v>
       </c>
@@ -11190,7 +11195,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1">
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>160</v>
       </c>
@@ -11220,7 +11225,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1">
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>160</v>
       </c>
@@ -11250,7 +11255,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1">
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>160</v>
       </c>
@@ -11280,7 +11285,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1">
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>160</v>
       </c>
@@ -11310,7 +11315,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1">
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>160</v>
       </c>
@@ -11340,7 +11345,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1">
+    <row r="133" spans="1:9">
       <c r="A133" t="s">
         <v>160</v>
       </c>
@@ -11370,7 +11375,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1">
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>160</v>
       </c>
@@ -11400,7 +11405,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1">
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>160</v>
       </c>
@@ -11430,7 +11435,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1">
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>160</v>
       </c>
@@ -11460,7 +11465,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1">
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>160</v>
       </c>
@@ -11490,7 +11495,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1">
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>160</v>
       </c>
@@ -11520,7 +11525,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1">
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>160</v>
       </c>
@@ -11550,7 +11555,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1">
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -11580,7 +11585,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1">
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>161</v>
       </c>
@@ -11610,7 +11615,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1">
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>161</v>
       </c>
@@ -11640,7 +11645,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1">
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -11670,7 +11675,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1">
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -11700,7 +11705,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1">
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>161</v>
       </c>
@@ -11730,7 +11735,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1">
+    <row r="146" spans="1:9">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -11760,7 +11765,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1">
+    <row r="147" spans="1:9">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -11790,7 +11795,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1">
+    <row r="148" spans="1:9">
       <c r="A148" t="s">
         <v>161</v>
       </c>
@@ -11820,7 +11825,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1">
+    <row r="149" spans="1:9">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -11850,7 +11855,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1">
+    <row r="150" spans="1:9">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -11880,7 +11885,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1">
+    <row r="151" spans="1:9">
       <c r="A151" t="s">
         <v>161</v>
       </c>
@@ -11910,7 +11915,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1">
+    <row r="152" spans="1:9">
       <c r="A152" t="s">
         <v>161</v>
       </c>
@@ -11940,7 +11945,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1">
+    <row r="153" spans="1:9">
       <c r="A153" t="s">
         <v>161</v>
       </c>
@@ -11970,7 +11975,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1">
+    <row r="154" spans="1:9">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -12000,7 +12005,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1">
+    <row r="155" spans="1:9">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -12030,7 +12035,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1">
+    <row r="156" spans="1:9">
       <c r="A156" t="s">
         <v>161</v>
       </c>
@@ -12060,7 +12065,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1">
+    <row r="157" spans="1:9">
       <c r="A157" t="s">
         <v>161</v>
       </c>
@@ -12090,7 +12095,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1">
+    <row r="158" spans="1:9">
       <c r="A158" t="s">
         <v>161</v>
       </c>
@@ -12120,7 +12125,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1">
+    <row r="159" spans="1:9">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -12150,7 +12155,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1">
+    <row r="160" spans="1:9">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -12180,7 +12185,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1">
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>161</v>
       </c>
@@ -12210,7 +12215,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1">
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -12240,7 +12245,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1">
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -12270,7 +12275,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1">
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>161</v>
       </c>
@@ -12300,7 +12305,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1">
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>170</v>
       </c>
@@ -12330,7 +12335,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1">
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>170</v>
       </c>
@@ -12339,7 +12344,7 @@
         <v>TelecommunicationsAppurtenanceTypeIMKLValue</v>
       </c>
       <c r="C166" t="s">
-        <v>954</v>
+        <v>137</v>
       </c>
       <c r="D166" t="s">
         <v>220</v>
@@ -12360,7 +12365,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1">
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -12390,7 +12395,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1">
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>338</v>
       </c>
@@ -12399,7 +12404,7 @@
         <v>TelecommunicationsCableMaterialTypeIMKLValue</v>
       </c>
       <c r="C168" t="s">
-        <v>958</v>
+        <v>1166</v>
       </c>
       <c r="D168" t="s">
         <v>176</v>
@@ -12420,7 +12425,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1">
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>338</v>
       </c>
@@ -12450,7 +12455,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1">
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>338</v>
       </c>
@@ -12480,7 +12485,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1">
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -12510,7 +12515,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1">
+    <row r="172" spans="1:9">
       <c r="A172" t="s">
         <v>327</v>
       </c>
@@ -12540,7 +12545,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1">
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>327</v>
       </c>
@@ -12570,7 +12575,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1">
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>327</v>
       </c>
@@ -12600,7 +12605,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1">
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>327</v>
       </c>
@@ -12630,7 +12635,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1">
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>325</v>
       </c>
@@ -12660,7 +12665,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1">
+    <row r="177" spans="1:9">
       <c r="A177" t="s">
         <v>325</v>
       </c>
@@ -12690,7 +12695,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1">
+    <row r="178" spans="1:9">
       <c r="A178" t="s">
         <v>325</v>
       </c>
@@ -12720,7 +12725,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1">
+    <row r="179" spans="1:9">
       <c r="A179" t="s">
         <v>325</v>
       </c>
@@ -12750,7 +12755,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1">
+    <row r="180" spans="1:9">
       <c r="A180" t="s">
         <v>320</v>
       </c>
@@ -12780,7 +12785,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1">
+    <row r="181" spans="1:9">
       <c r="A181" t="s">
         <v>320</v>
       </c>
@@ -12810,7 +12815,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1">
+    <row r="182" spans="1:9">
       <c r="A182" t="s">
         <v>320</v>
       </c>
@@ -12840,7 +12845,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1">
+    <row r="183" spans="1:9">
       <c r="A183" t="s">
         <v>320</v>
       </c>
@@ -12870,7 +12875,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1">
+    <row r="184" spans="1:9">
       <c r="A184" t="s">
         <v>341</v>
       </c>
@@ -12900,7 +12905,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="28.8" hidden="1">
+    <row r="185" spans="1:9" ht="28.8">
       <c r="A185" t="s">
         <v>323</v>
       </c>
@@ -12930,7 +12935,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1">
+    <row r="186" spans="1:9">
       <c r="A186" t="s">
         <v>158</v>
       </c>
@@ -12960,7 +12965,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="57.6" hidden="1">
+    <row r="187" spans="1:9" ht="57.6">
       <c r="A187" t="s">
         <v>323</v>
       </c>
@@ -12990,7 +12995,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1">
+    <row r="188" spans="1:9">
       <c r="A188" t="s">
         <v>315</v>
       </c>
@@ -13020,7 +13025,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="189" spans="1:9" hidden="1">
+    <row r="189" spans="1:9">
       <c r="A189" t="s">
         <v>315</v>
       </c>
@@ -13050,7 +13055,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1">
+    <row r="190" spans="1:9">
       <c r="A190" t="s">
         <v>316</v>
       </c>
@@ -13080,7 +13085,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1">
+    <row r="191" spans="1:9">
       <c r="A191" t="s">
         <v>316</v>
       </c>
@@ -13110,7 +13115,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1">
+    <row r="192" spans="1:9">
       <c r="A192" t="s">
         <v>316</v>
       </c>
@@ -13140,7 +13145,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1">
+    <row r="193" spans="1:9">
       <c r="A193" t="s">
         <v>317</v>
       </c>
@@ -13170,7 +13175,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1">
+    <row r="194" spans="1:9">
       <c r="A194" t="s">
         <v>317</v>
       </c>
@@ -13200,7 +13205,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1">
+    <row r="195" spans="1:9">
       <c r="A195" t="s">
         <v>152</v>
       </c>
@@ -13230,7 +13235,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1">
+    <row r="196" spans="1:9">
       <c r="A196" t="s">
         <v>317</v>
       </c>
@@ -13260,7 +13265,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1">
+    <row r="197" spans="1:9">
       <c r="A197" t="s">
         <v>317</v>
       </c>
@@ -13290,7 +13295,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1">
+    <row r="198" spans="1:9">
       <c r="A198" t="s">
         <v>317</v>
       </c>
@@ -13320,7 +13325,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1">
+    <row r="199" spans="1:9">
       <c r="A199" t="s">
         <v>318</v>
       </c>
@@ -13350,7 +13355,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1">
+    <row r="200" spans="1:9">
       <c r="A200" t="s">
         <v>318</v>
       </c>
@@ -13380,7 +13385,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1">
+    <row r="201" spans="1:9">
       <c r="A201" t="s">
         <v>318</v>
       </c>
@@ -13410,7 +13415,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1">
+    <row r="202" spans="1:9">
       <c r="A202" t="s">
         <v>318</v>
       </c>
@@ -13440,7 +13445,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1">
+    <row r="203" spans="1:9">
       <c r="A203" t="s">
         <v>318</v>
       </c>
@@ -13470,7 +13475,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1">
+    <row r="204" spans="1:9">
       <c r="A204" t="s">
         <v>318</v>
       </c>
@@ -13500,7 +13505,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1">
+    <row r="205" spans="1:9">
       <c r="A205" t="s">
         <v>318</v>
       </c>
@@ -13530,7 +13535,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1">
+    <row r="206" spans="1:9">
       <c r="A206" t="s">
         <v>318</v>
       </c>
@@ -13560,7 +13565,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1">
+    <row r="207" spans="1:9">
       <c r="A207" t="s">
         <v>318</v>
       </c>
@@ -13590,7 +13595,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1">
+    <row r="208" spans="1:9">
       <c r="A208" t="s">
         <v>318</v>
       </c>
@@ -13620,7 +13625,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="209" spans="1:9" hidden="1">
+    <row r="209" spans="1:9">
       <c r="A209" t="s">
         <v>318</v>
       </c>
@@ -13650,7 +13655,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1">
+    <row r="210" spans="1:9">
       <c r="A210" t="s">
         <v>170</v>
       </c>
@@ -13680,7 +13685,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1">
+    <row r="211" spans="1:9">
       <c r="A211" t="s">
         <v>170</v>
       </c>
@@ -13689,7 +13694,7 @@
         <v>TelecommunicationsAppurtenanceTypeIMKLValue</v>
       </c>
       <c r="C211" t="s">
-        <v>956</v>
+        <v>1165</v>
       </c>
       <c r="D211" t="s">
         <v>221</v>
@@ -13710,7 +13715,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1">
+    <row r="212" spans="1:9">
       <c r="A212" t="s">
         <v>322</v>
       </c>
@@ -13740,7 +13745,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1">
+    <row r="213" spans="1:9">
       <c r="A213" t="s">
         <v>322</v>
       </c>
@@ -13770,7 +13775,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="214" spans="1:9" hidden="1">
+    <row r="214" spans="1:9">
       <c r="A214" t="s">
         <v>322</v>
       </c>
@@ -13800,7 +13805,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1">
+    <row r="215" spans="1:9">
       <c r="A215" t="s">
         <v>322</v>
       </c>
@@ -13830,7 +13835,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="216" spans="1:9" hidden="1">
+    <row r="216" spans="1:9">
       <c r="A216" t="s">
         <v>322</v>
       </c>
@@ -13860,7 +13865,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="217" spans="1:9" hidden="1">
+    <row r="217" spans="1:9">
       <c r="A217" t="s">
         <v>322</v>
       </c>
@@ -13890,7 +13895,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1">
+    <row r="218" spans="1:9">
       <c r="A218" t="s">
         <v>340</v>
       </c>
@@ -13920,7 +13925,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="219" spans="1:9" hidden="1">
+    <row r="219" spans="1:9">
       <c r="A219" t="s">
         <v>173</v>
       </c>
@@ -13950,7 +13955,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1">
+    <row r="220" spans="1:9">
       <c r="A220" t="s">
         <v>173</v>
       </c>
@@ -13980,7 +13985,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1">
+    <row r="221" spans="1:9">
       <c r="A221" t="s">
         <v>173</v>
       </c>
@@ -14010,7 +14015,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1">
+    <row r="222" spans="1:9">
       <c r="A222" t="s">
         <v>6</v>
       </c>
@@ -14040,7 +14045,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1">
+    <row r="223" spans="1:9">
       <c r="A223" t="s">
         <v>6</v>
       </c>
@@ -14070,7 +14075,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1">
+    <row r="224" spans="1:9">
       <c r="A224" t="s">
         <v>6</v>
       </c>
@@ -14100,7 +14105,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1">
+    <row r="225" spans="1:9">
       <c r="A225" t="s">
         <v>6</v>
       </c>
@@ -14130,7 +14135,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1">
+    <row r="226" spans="1:9">
       <c r="A226" t="s">
         <v>241</v>
       </c>
@@ -14160,7 +14165,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1">
+    <row r="227" spans="1:9">
       <c r="A227" t="s">
         <v>241</v>
       </c>
@@ -14190,7 +14195,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1">
+    <row r="228" spans="1:9">
       <c r="A228" t="s">
         <v>241</v>
       </c>
@@ -14220,7 +14225,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1">
+    <row r="229" spans="1:9">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -14241,7 +14246,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1">
+    <row r="230" spans="1:9">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -14262,7 +14267,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1">
+    <row r="231" spans="1:9">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -14283,7 +14288,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1">
+    <row r="232" spans="1:9">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -14304,7 +14309,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1">
+    <row r="233" spans="1:9">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -14325,7 +14330,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1">
+    <row r="234" spans="1:9">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -14355,7 +14360,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1">
+    <row r="235" spans="1:9">
       <c r="A235" t="s">
         <v>10</v>
       </c>
@@ -14385,7 +14390,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1">
+    <row r="236" spans="1:9">
       <c r="A236" t="s">
         <v>10</v>
       </c>
@@ -14415,7 +14420,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1">
+    <row r="237" spans="1:9">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -14445,7 +14450,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1">
+    <row r="238" spans="1:9">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -14475,7 +14480,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1">
+    <row r="239" spans="1:9">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -14505,7 +14510,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1">
+    <row r="240" spans="1:9">
       <c r="A240" t="s">
         <v>10</v>
       </c>
@@ -14535,7 +14540,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1">
+    <row r="241" spans="1:9">
       <c r="A241" t="s">
         <v>10</v>
       </c>
@@ -14565,7 +14570,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1">
+    <row r="242" spans="1:9">
       <c r="A242" t="s">
         <v>10</v>
       </c>
@@ -14595,7 +14600,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1">
+    <row r="243" spans="1:9">
       <c r="A243" t="s">
         <v>10</v>
       </c>
@@ -14625,7 +14630,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1">
+    <row r="244" spans="1:9">
       <c r="A244" t="s">
         <v>8</v>
       </c>
@@ -14655,7 +14660,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1">
+    <row r="245" spans="1:9">
       <c r="A245" t="s">
         <v>8</v>
       </c>
@@ -14685,7 +14690,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1">
+    <row r="246" spans="1:9">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -14715,7 +14720,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1">
+    <row r="247" spans="1:9">
       <c r="A247" t="s">
         <v>258</v>
       </c>
@@ -14745,7 +14750,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1">
+    <row r="248" spans="1:9">
       <c r="A248" t="s">
         <v>258</v>
       </c>
@@ -14775,7 +14780,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1">
+    <row r="249" spans="1:9">
       <c r="A249" t="s">
         <v>258</v>
       </c>
@@ -14805,7 +14810,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1">
+    <row r="250" spans="1:9">
       <c r="A250" t="s">
         <v>258</v>
       </c>
@@ -14836,18 +14841,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="ElectricitySubthemeValue"/>
-        <filter val="OilGasChemicalsSubthemeValue"/>
-        <filter val="SewerSubthemeValue"/>
-        <filter val="TelecommunicationsSubthemeValue"/>
-        <filter val="ThermalSubthemeValue"/>
-        <filter val="WaterSubthemeValue"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I250" xr:uid="{75ABF075-1189-4C98-A20B-91C63C9C478D}"/>
   <hyperlinks>
     <hyperlink ref="H180" r:id="rId1" xr:uid="{937649D5-206B-4F0F-AC39-B248CB8B3379}"/>
     <hyperlink ref="H215" r:id="rId2" xr:uid="{58EA29A0-45FB-4990-9EF7-62E6622DF2D7}"/>
@@ -14907,6 +14901,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088F26AC8FFACDA459ED97BA33A2EDD09" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d100541493c99754ab38f69507ec9314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dbdd298-def3-48d5-b10a-519f5ec7909f" xmlns:ns3="b7ca5a17-62b2-45ee-a209-788463db48b0" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f133327a4eb5a6191fb38303f059c04" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6dbdd298-def3-48d5-b10a-519f5ec7909f"/>
@@ -15166,16 +15169,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{791B434E-C5B6-43DF-B218-859297235BBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15193,12 +15195,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DC2C1C4-4794-4CDA-B113-FDC4260BCF94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>